<commit_message>
Ajout de trucs dans analyse et SLAP
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annie\Desktop\Technique Informatique\UML\TPFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annie\Desktop\Technique Informatique\UML\TPfinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Coût de développement</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Réduction de frais lié au personnel</t>
+  </si>
+  <si>
+    <t>Période de récupération</t>
+  </si>
+  <si>
+    <t>Avantages-Investissement</t>
+  </si>
+  <si>
+    <t>Investissement</t>
+  </si>
+  <si>
+    <t>Rendement du capital investi sur 5 ans</t>
   </si>
 </sst>
 </file>
@@ -162,11 +174,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -181,10 +194,13 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D927E1A-B0F7-449E-B86D-CCB5AC63D3B9}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,6 +812,41 @@
         <v>85048.050000000017</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="12">
+        <f>G27</f>
+        <v>85048.050000000017</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="12">
+        <f>-(B24+C25+D25+E25+F25+G25)</f>
+        <v>70771.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="13">
+        <f>B30/B31</f>
+        <v>1.2017197491379004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>